<commit_message>
Updated with data till 1st June 2024
</commit_message>
<xml_diff>
--- a/Turf Treckers.xlsx
+++ b/Turf Treckers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b5b54234053f92f7/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Cricket\Cricket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="796" documentId="8_{E6D1E935-DCA2-47C9-8D0C-B2510630F00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D53934B7-99B7-404E-BD02-119880ABD051}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B589B24D-6CE7-4F1A-B271-B61B31E4D41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{F1DA30EA-0585-4EF8-A8EC-5016E264CAF2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -85,15 +85,9 @@
     <t>Shahul</t>
   </si>
   <si>
-    <t>18*</t>
-  </si>
-  <si>
     <t>Harish</t>
   </si>
   <si>
-    <t>Sridhar</t>
-  </si>
-  <si>
     <t>Santhosh</t>
   </si>
   <si>
@@ -109,9 +103,6 @@
     <t>Bala</t>
   </si>
   <si>
-    <t>27*</t>
-  </si>
-  <si>
     <t>33*</t>
   </si>
   <si>
@@ -154,9 +145,6 @@
     <t>2/0</t>
   </si>
   <si>
-    <t>Imran</t>
-  </si>
-  <si>
     <t>Jain</t>
   </si>
   <si>
@@ -169,21 +157,12 @@
     <t>Jai</t>
   </si>
   <si>
-    <t>2/1</t>
-  </si>
-  <si>
-    <t>2/2</t>
-  </si>
-  <si>
     <t>3/9</t>
   </si>
   <si>
     <t>3/0</t>
   </si>
   <si>
-    <t>3/21</t>
-  </si>
-  <si>
     <t>Yusuf</t>
   </si>
   <si>
@@ -209,6 +188,21 @@
   </si>
   <si>
     <t>Total Impressions</t>
+  </si>
+  <si>
+    <t>42*</t>
+  </si>
+  <si>
+    <t>34*</t>
+  </si>
+  <si>
+    <t>Boo</t>
+  </si>
+  <si>
+    <t>Arvindh</t>
+  </si>
+  <si>
+    <t>30*</t>
   </si>
 </sst>
 </file>
@@ -288,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -299,6 +293,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -316,14 +313,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -361,7 +354,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -467,7 +460,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -609,7 +602,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -620,7 +613,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -662,107 +655,107 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B2">
-        <v>94</v>
+        <v>180</v>
       </c>
       <c r="C2">
-        <v>86</v>
+        <v>166</v>
       </c>
       <c r="D2">
-        <v>1039</v>
+        <v>2173</v>
       </c>
       <c r="E2">
         <v>52</v>
       </c>
       <c r="F2">
-        <v>18.89</v>
+        <v>19.75</v>
       </c>
       <c r="G2">
-        <v>103.28</v>
+        <v>117.91</v>
       </c>
       <c r="H2">
-        <v>80</v>
+        <v>193</v>
       </c>
       <c r="I2">
-        <v>81</v>
+        <v>155</v>
       </c>
       <c r="J2">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B3">
-        <v>87</v>
+        <v>187</v>
       </c>
       <c r="C3">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="D3">
-        <v>641</v>
+        <v>1391</v>
       </c>
       <c r="E3" s="1">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="F3">
-        <v>12.57</v>
+        <v>10.3</v>
       </c>
       <c r="G3">
-        <v>94.96</v>
+        <v>109.87</v>
       </c>
       <c r="H3">
-        <v>49</v>
+        <v>133</v>
       </c>
       <c r="I3">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4">
-        <v>89</v>
+        <v>171</v>
       </c>
       <c r="C4">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="D4">
-        <v>603</v>
+        <v>1332</v>
       </c>
       <c r="E4" s="1">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="F4">
-        <v>9.14</v>
+        <v>13.06</v>
       </c>
       <c r="G4">
-        <v>103.97</v>
+        <v>98.96</v>
       </c>
       <c r="H4">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="I4">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="J4">
         <v>3</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -770,66 +763,66 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>87</v>
+        <v>156</v>
       </c>
       <c r="C5">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="D5">
-        <v>575</v>
+        <v>1068</v>
       </c>
       <c r="E5" s="1">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="F5">
-        <v>9.91</v>
+        <v>10.17</v>
       </c>
       <c r="G5">
-        <v>91.71</v>
+        <v>97.45</v>
       </c>
       <c r="H5">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="I5">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
         <v>1</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B6">
-        <v>91</v>
+        <v>152</v>
       </c>
       <c r="C6">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="D6">
-        <v>482</v>
+        <v>1037</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="F6">
-        <v>8.61</v>
+        <v>12.8</v>
       </c>
       <c r="G6">
-        <v>102.77</v>
+        <v>115.61</v>
       </c>
       <c r="H6">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="I6">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -837,34 +830,34 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>77</v>
+        <v>207</v>
       </c>
       <c r="C7">
-        <v>63</v>
+        <v>178</v>
       </c>
       <c r="D7">
-        <v>451</v>
+        <v>1005</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F7">
-        <v>13.26</v>
+        <v>8.31</v>
       </c>
       <c r="G7">
-        <v>95.55</v>
+        <v>92.46</v>
       </c>
       <c r="H7">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="I7">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="J7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -872,34 +865,34 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B8">
-        <v>74</v>
+        <v>135</v>
       </c>
       <c r="C8">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="D8">
-        <v>415</v>
+        <v>948</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F8">
-        <v>10.119999999999999</v>
+        <v>14.81</v>
       </c>
       <c r="G8">
-        <v>105.06</v>
+        <v>108.22</v>
       </c>
       <c r="H8">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="I8">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="J8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -910,31 +903,31 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="C9">
-        <v>61</v>
+        <v>133</v>
       </c>
       <c r="D9">
-        <v>342</v>
+        <v>942</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F9">
-        <v>8.77</v>
+        <v>12.39</v>
       </c>
       <c r="G9">
-        <v>73.23</v>
+        <v>94.77</v>
       </c>
       <c r="H9">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="I9">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -942,34 +935,34 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10">
-        <v>56</v>
+        <v>133</v>
       </c>
       <c r="C10">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="D10">
-        <v>311</v>
+        <v>637</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F10">
-        <v>10.37</v>
+        <v>9.23</v>
       </c>
       <c r="G10">
-        <v>100.32</v>
+        <v>103.58</v>
       </c>
       <c r="H10">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="I10">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -977,34 +970,34 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="B11">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C11">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D11">
-        <v>285</v>
-      </c>
-      <c r="E11">
-        <v>27</v>
+        <v>526</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="F11">
-        <v>7.13</v>
+        <v>11.43</v>
       </c>
       <c r="G11">
-        <v>85.59</v>
+        <v>111.91</v>
       </c>
       <c r="H11">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="I11">
         <v>15</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1019,7 +1012,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD3E505-BD2B-4338-A86B-6E0D13799BD4}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1034,28 +1029,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>6</v>
@@ -1064,325 +1059,325 @@
         <v>5</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B2">
-        <v>77</v>
+        <v>156</v>
       </c>
       <c r="C2">
-        <v>70</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="E2" s="6">
-        <v>9</v>
+        <v>154</v>
+      </c>
+      <c r="D2" s="6">
+        <v>194.5</v>
+      </c>
+      <c r="E2">
+        <v>11</v>
       </c>
       <c r="F2">
-        <v>465</v>
+        <v>1062</v>
       </c>
       <c r="G2" s="6">
-        <v>52</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="6">
+        <v>2</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
-      <c r="K2" s="6">
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="L2" s="6">
-        <v>11.54</v>
-      </c>
-      <c r="M2" s="6">
-        <v>8.94</v>
-      </c>
-      <c r="N2" s="6">
-        <v>32</v>
-      </c>
-      <c r="O2" s="6">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>394</v>
+      <c r="K2">
+        <v>5.46</v>
+      </c>
+      <c r="L2">
+        <v>14.08</v>
+      </c>
+      <c r="M2">
+        <v>12.78</v>
+      </c>
+      <c r="N2">
+        <v>157</v>
+      </c>
+      <c r="O2">
+        <v>11</v>
+      </c>
+      <c r="P2" s="6">
+        <v>745</v>
       </c>
       <c r="Q2">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="R2">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>135</v>
+      </c>
+      <c r="C3">
+        <v>124</v>
+      </c>
+      <c r="D3">
+        <v>164.2</v>
+      </c>
+      <c r="E3" s="6">
         <v>13</v>
       </c>
-      <c r="B3">
-        <v>87</v>
-      </c>
-      <c r="C3" s="6">
-        <v>86</v>
-      </c>
-      <c r="D3" s="6">
-        <v>124.5</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
       <c r="F3">
-        <v>687</v>
-      </c>
-      <c r="G3">
-        <v>44</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="6">
-        <v>2</v>
+        <v>892</v>
+      </c>
+      <c r="G3" s="8">
+        <v>71</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
-      <c r="K3">
-        <v>5.52</v>
+      <c r="K3" s="6">
+        <v>5.43</v>
       </c>
       <c r="L3">
-        <v>16.89</v>
-      </c>
-      <c r="M3">
-        <v>15.61</v>
-      </c>
-      <c r="N3">
-        <v>93</v>
-      </c>
-      <c r="O3">
-        <v>7</v>
-      </c>
-      <c r="P3" s="6">
-        <v>457</v>
+        <v>13.89</v>
+      </c>
+      <c r="M3" s="6">
+        <v>12.56</v>
+      </c>
+      <c r="N3" s="6">
+        <v>51</v>
+      </c>
+      <c r="O3" s="6">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>598</v>
       </c>
       <c r="Q3">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="R3">
-        <v>42</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>74</v>
+        <v>174</v>
       </c>
       <c r="C4">
-        <v>70</v>
+        <v>147</v>
       </c>
       <c r="D4">
-        <v>79.2</v>
+        <v>144.1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F4">
-        <v>433</v>
+        <v>1066</v>
       </c>
       <c r="G4">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>5.47</v>
+        <v>7.4</v>
       </c>
       <c r="L4">
-        <v>14.88</v>
+        <v>13.52</v>
       </c>
       <c r="M4">
-        <v>13.53</v>
+        <v>16.66</v>
       </c>
       <c r="N4">
-        <v>68</v>
+        <v>114</v>
       </c>
       <c r="O4">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="P4">
-        <v>284</v>
+        <v>501</v>
       </c>
       <c r="Q4">
-        <v>24</v>
-      </c>
-      <c r="R4" s="6">
-        <v>19</v>
+        <v>52</v>
+      </c>
+      <c r="R4">
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B5">
-        <v>87</v>
+        <v>187</v>
       </c>
       <c r="C5">
-        <v>82</v>
+        <v>134</v>
       </c>
       <c r="D5">
-        <v>104.1</v>
+        <v>127.3</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>667</v>
+        <v>1141</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>6.41</v>
-      </c>
-      <c r="L5">
-        <v>20.83</v>
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="L5" s="6">
+        <v>12.75</v>
       </c>
       <c r="M5">
-        <v>22.23</v>
+        <v>19.02</v>
       </c>
       <c r="N5">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="O5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="P5">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="Q5">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="R5">
-        <v>39</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6">
-        <v>60</v>
+        <v>152</v>
       </c>
       <c r="C6">
-        <v>54</v>
+        <v>145</v>
       </c>
       <c r="D6">
-        <v>85</v>
+        <v>156.4</v>
       </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>960</v>
+      </c>
+      <c r="G6">
+        <v>59</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6">
         <v>1</v>
       </c>
-      <c r="F6">
-        <v>630</v>
-      </c>
-      <c r="G6">
-        <v>30</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" s="6">
-        <v>2</v>
-      </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>7.41</v>
+        <v>6.14</v>
       </c>
       <c r="L6">
-        <v>17</v>
+        <v>15.93</v>
       </c>
       <c r="M6">
-        <v>21</v>
+        <v>16.27</v>
       </c>
       <c r="N6">
-        <v>80</v>
+        <v>149</v>
       </c>
       <c r="O6">
         <v>6</v>
       </c>
       <c r="P6">
-        <v>266</v>
+        <v>562</v>
       </c>
       <c r="Q6">
-        <v>51</v>
-      </c>
-      <c r="R6">
-        <v>22</v>
+        <v>49</v>
+      </c>
+      <c r="R6" s="6">
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B7">
-        <v>60</v>
+        <v>171</v>
       </c>
       <c r="C7">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D7">
-        <v>75.2</v>
+        <v>185.4</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>482</v>
+        <v>1259</v>
       </c>
       <c r="G7">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -1391,110 +1386,110 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>6.41</v>
+        <v>6.79</v>
       </c>
       <c r="L7">
-        <v>16.14</v>
+        <v>18.88</v>
       </c>
       <c r="M7">
-        <v>17.21</v>
+        <v>21.34</v>
       </c>
       <c r="N7">
-        <v>66</v>
-      </c>
-      <c r="O7" s="6">
-        <v>0</v>
+        <v>191</v>
+      </c>
+      <c r="O7">
+        <v>13</v>
       </c>
       <c r="P7">
-        <v>261</v>
+        <v>666</v>
       </c>
       <c r="Q7">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="R7">
-        <v>30</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B8">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="C8">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="D8">
-        <v>65.2</v>
+        <v>134.1</v>
       </c>
       <c r="E8">
         <v>4</v>
       </c>
       <c r="F8">
-        <v>456</v>
+        <v>894</v>
       </c>
       <c r="G8">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <v>6.99</v>
+        <v>6.67</v>
       </c>
       <c r="L8">
-        <v>14</v>
+        <v>14.38</v>
       </c>
       <c r="M8">
-        <v>16.29</v>
+        <v>15.96</v>
       </c>
       <c r="N8">
-        <v>38</v>
-      </c>
-      <c r="O8">
-        <v>10</v>
+        <v>123</v>
+      </c>
+      <c r="O8" s="6">
+        <v>0</v>
       </c>
       <c r="P8">
-        <v>232</v>
+        <v>473</v>
       </c>
       <c r="Q8">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="R8">
-        <v>33</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B9" s="6">
-        <v>94</v>
-      </c>
-      <c r="C9">
-        <v>85</v>
+        <v>180</v>
+      </c>
+      <c r="C9" s="6">
+        <v>164</v>
       </c>
       <c r="D9">
-        <v>87.3</v>
+        <v>167.4</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F9">
-        <v>535</v>
+        <v>1073</v>
       </c>
       <c r="G9">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1503,140 +1498,140 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>6.13</v>
+        <v>6.41</v>
       </c>
       <c r="L9">
-        <v>21.63</v>
+        <v>18.63</v>
       </c>
       <c r="M9">
-        <v>22.29</v>
+        <v>19.87</v>
       </c>
       <c r="N9">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="O9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="P9">
-        <v>308</v>
+        <v>607</v>
       </c>
       <c r="Q9">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="R9">
-        <v>36</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B10">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="C10">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="D10">
-        <v>54.5</v>
+        <v>99.2</v>
       </c>
       <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>741</v>
+      </c>
+      <c r="G10">
+        <v>43</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10">
         <v>1</v>
       </c>
-      <c r="F10">
-        <v>385</v>
-      </c>
-      <c r="G10">
-        <v>24</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>7.06</v>
+        <v>7.47</v>
       </c>
       <c r="L10">
-        <v>13.46</v>
+        <v>13.86</v>
       </c>
       <c r="M10">
-        <v>16.04</v>
+        <v>17.23</v>
       </c>
       <c r="N10">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="O10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P10">
-        <v>204</v>
+        <v>373</v>
       </c>
       <c r="Q10" s="6">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="R10">
-        <v>31</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="B11">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="C11">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="D11">
+        <v>77.3</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>684</v>
+      </c>
+      <c r="G11">
+        <v>38</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>8.85</v>
+      </c>
+      <c r="L11">
+        <v>12.24</v>
+      </c>
+      <c r="M11">
+        <v>18</v>
+      </c>
+      <c r="N11">
+        <v>69</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="P11">
+        <v>251</v>
+      </c>
+      <c r="Q11">
+        <v>33</v>
+      </c>
+      <c r="R11">
         <v>59</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
-      <c r="F11">
-        <v>395</v>
-      </c>
-      <c r="G11">
-        <v>21</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>6.69</v>
-      </c>
-      <c r="L11">
-        <v>16.86</v>
-      </c>
-      <c r="M11">
-        <v>18.809999999999999</v>
-      </c>
-      <c r="N11">
-        <v>38</v>
-      </c>
-      <c r="O11">
-        <v>4</v>
-      </c>
-      <c r="P11">
-        <v>201</v>
-      </c>
-      <c r="Q11" s="6">
-        <v>16</v>
-      </c>
-      <c r="R11">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1650,7 +1645,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1669,49 +1664,49 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B2">
-        <v>94</v>
+        <v>180</v>
       </c>
       <c r="C2" s="7">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2">
-        <v>21</v>
+      <c r="E2" s="7">
+        <v>38</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H2" s="7">
         <f>SUM(C2:G2)</f>
-        <v>58</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -1719,43 +1714,43 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="C3">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>22</v>
+      <c r="E3" s="7">
+        <v>38</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H12" si="0">SUM(C3:G3)</f>
-        <v>54</v>
+        <f t="shared" ref="H3:H11" si="0">SUM(C3:G3)</f>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>77</v>
+        <v>135</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" s="7">
-        <v>24</v>
+      <c r="E4">
+        <v>35</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1765,196 +1760,196 @@
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B5">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5" s="7">
+        <v>32</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>37</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
         <v>4</v>
       </c>
-      <c r="E5">
-        <v>8</v>
-      </c>
-      <c r="F5" s="7">
-        <v>8</v>
-      </c>
-      <c r="G5" s="7">
-        <v>10</v>
-      </c>
       <c r="H5">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f>SUM(C5:G5)</f>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>56</v>
+        <v>187</v>
       </c>
       <c r="C6">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="D6" s="7">
+        <v>9</v>
       </c>
       <c r="E6">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F6" s="7">
-        <v>8</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="G6" s="7">
+        <v>17</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B7">
-        <v>74</v>
+        <v>152</v>
       </c>
       <c r="C7">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8">
-        <v>87</v>
+        <v>207</v>
       </c>
       <c r="C8">
         <v>19</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8">
+        <v>28</v>
+      </c>
+      <c r="F8">
         <v>6</v>
       </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
       <c r="G8">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <f>SUM(C8:G8)</f>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9">
-        <v>87</v>
+        <v>171</v>
       </c>
       <c r="C9">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>15</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>23</v>
+      </c>
+      <c r="F10">
         <v>1</v>
       </c>
-      <c r="E10">
-        <v>13</v>
-      </c>
-      <c r="F10">
-        <v>4</v>
-      </c>
       <c r="G10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B11">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>